<commit_message>
Add Push Signal To Excel Sheet
</commit_message>
<xml_diff>
--- a/docs/ControlUnit.xlsx
+++ b/docs/ControlUnit.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\ar-kak-tecture\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA0C600F-02C5-49C5-90DA-2DEDB5DEDCC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6271E955-A253-4700-917E-1DC59C57AA2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{447A83B7-4152-47C5-88BB-EC7BDAAC407E}"/>
   </bookViews>
@@ -158,10 +158,10 @@
     <t>x</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Fitch/Decode Signa</t>
+  </si>
+  <si>
+    <t>Push</t>
   </si>
 </sst>
 </file>
@@ -708,7 +708,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -870,19 +870,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -900,12 +900,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -918,47 +912,47 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1277,7 +1271,7 @@
   <dimension ref="A1:AJ31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1290,19 +1284,20 @@
     <col min="16" max="16" width="13.88671875" style="1" customWidth="1"/>
     <col min="17" max="17" width="12.77734375" customWidth="1"/>
     <col min="18" max="18" width="22.44140625" customWidth="1"/>
+    <col min="21" max="21" width="23.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" s="2" customFormat="1" ht="28.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="79" t="s">
+      <c r="B1" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="81"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="71"/>
       <c r="G1" s="62" t="s">
         <v>8</v>
       </c>
@@ -1310,20 +1305,17 @@
       <c r="I1" s="63"/>
       <c r="J1" s="63"/>
       <c r="K1" s="63"/>
-      <c r="L1" s="64"/>
-      <c r="N1" s="65" t="s">
+      <c r="L1" s="63"/>
+      <c r="M1" s="64"/>
+      <c r="Q1" s="72" t="s">
         <v>34</v>
       </c>
-      <c r="O1" s="66"/>
-      <c r="P1" s="67" t="s">
+      <c r="R1" s="74"/>
+      <c r="S1" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="Q1" s="68"/>
-      <c r="R1" s="69"/>
-      <c r="S1"/>
-      <c r="T1"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
+      <c r="T1" s="66"/>
+      <c r="U1" s="67"/>
       <c r="X1" s="3"/>
       <c r="Y1" s="3"/>
       <c r="Z1" s="3"/>
@@ -1340,11 +1332,11 @@
     </row>
     <row r="2" spans="1:36" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="61"/>
-      <c r="B2" s="82"/>
-      <c r="C2" s="83"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="84"/>
+      <c r="B2" s="72"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="74"/>
       <c r="G2" s="30" t="s">
         <v>9</v>
       </c>
@@ -1360,25 +1352,25 @@
       <c r="K2" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="L2" s="32" t="s">
+      <c r="L2" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="M2" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="N2" s="53" t="s">
+      <c r="Q2" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="O2" s="53" t="s">
+      <c r="R2" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="P2" s="55" t="s">
+      <c r="S2" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="Q2" s="56" t="s">
+      <c r="T2" s="55" t="s">
         <v>35</v>
       </c>
-      <c r="R2" s="56" t="s">
-        <v>42</v>
-      </c>
-      <c r="S2" t="s">
+      <c r="U2" s="55" t="s">
         <v>41</v>
       </c>
       <c r="X2" s="1"/>
@@ -1429,22 +1421,25 @@
       <c r="K3" s="18">
         <v>0</v>
       </c>
-      <c r="L3" s="32">
-        <v>0</v>
-      </c>
-      <c r="N3" s="12">
-        <v>0</v>
-      </c>
-      <c r="O3" s="12">
-        <v>0</v>
-      </c>
-      <c r="P3" s="59">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="57">
-        <v>0</v>
-      </c>
-      <c r="R3" s="57"/>
+      <c r="L3" s="18">
+        <v>0</v>
+      </c>
+      <c r="M3" s="32">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="12">
+        <v>0</v>
+      </c>
+      <c r="R3" s="12">
+        <v>0</v>
+      </c>
+      <c r="S3" s="58">
+        <v>0</v>
+      </c>
+      <c r="T3" s="56">
+        <v>0</v>
+      </c>
+      <c r="U3" s="56"/>
       <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
@@ -1493,22 +1488,25 @@
       <c r="K4" s="18">
         <v>0</v>
       </c>
-      <c r="L4" s="32">
-        <v>0</v>
-      </c>
-      <c r="N4" s="12">
-        <v>0</v>
-      </c>
-      <c r="O4" s="12">
-        <v>1</v>
-      </c>
-      <c r="P4" s="57">
-        <v>1</v>
-      </c>
-      <c r="Q4" s="57">
-        <v>0</v>
-      </c>
-      <c r="R4" s="57"/>
+      <c r="L4" s="18">
+        <v>0</v>
+      </c>
+      <c r="M4" s="32">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="12">
+        <v>0</v>
+      </c>
+      <c r="R4" s="12">
+        <v>1</v>
+      </c>
+      <c r="S4" s="56">
+        <v>1</v>
+      </c>
+      <c r="T4" s="56">
+        <v>0</v>
+      </c>
+      <c r="U4" s="56"/>
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
@@ -1557,22 +1555,25 @@
       <c r="K5" s="18">
         <v>0</v>
       </c>
-      <c r="L5" s="32">
-        <v>0</v>
-      </c>
-      <c r="N5" s="12">
-        <v>1</v>
-      </c>
-      <c r="O5" s="12">
-        <v>0</v>
-      </c>
-      <c r="P5" s="57">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="57">
-        <v>1</v>
-      </c>
-      <c r="R5" s="57"/>
+      <c r="L5" s="18">
+        <v>0</v>
+      </c>
+      <c r="M5" s="32">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="12">
+        <v>1</v>
+      </c>
+      <c r="R5" s="12">
+        <v>0</v>
+      </c>
+      <c r="S5" s="56">
+        <v>1</v>
+      </c>
+      <c r="T5" s="56">
+        <v>1</v>
+      </c>
+      <c r="U5" s="56"/>
       <c r="X5" s="1"/>
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
@@ -1621,22 +1622,25 @@
       <c r="K6" s="18">
         <v>0</v>
       </c>
-      <c r="L6" s="32">
-        <v>0</v>
-      </c>
-      <c r="N6" s="51">
-        <v>1</v>
-      </c>
-      <c r="O6" s="52">
-        <v>1</v>
-      </c>
-      <c r="P6" s="54" t="s">
+      <c r="L6" s="18">
+        <v>0</v>
+      </c>
+      <c r="M6" s="32">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="51">
+        <v>1</v>
+      </c>
+      <c r="R6" s="52">
+        <v>1</v>
+      </c>
+      <c r="S6" s="54" t="s">
         <v>40</v>
       </c>
-      <c r="Q6" s="58" t="s">
+      <c r="T6" s="57" t="s">
         <v>40</v>
       </c>
-      <c r="R6" s="58"/>
+      <c r="U6" s="57"/>
       <c r="X6" s="1"/>
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
@@ -1685,10 +1689,12 @@
       <c r="K7" s="18">
         <v>0</v>
       </c>
-      <c r="L7" s="32">
-        <v>0</v>
-      </c>
-      <c r="P7"/>
+      <c r="L7" s="18">
+        <v>0</v>
+      </c>
+      <c r="M7" s="32">
+        <v>0</v>
+      </c>
       <c r="X7" s="1"/>
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
@@ -1737,9 +1743,13 @@
       <c r="K8" s="18">
         <v>0</v>
       </c>
-      <c r="L8" s="32">
-        <v>0</v>
-      </c>
+      <c r="L8" s="18">
+        <v>0</v>
+      </c>
+      <c r="M8" s="32">
+        <v>0</v>
+      </c>
+      <c r="S8" s="1"/>
       <c r="X8" s="1"/>
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
@@ -1788,9 +1798,13 @@
       <c r="K9" s="17">
         <v>0</v>
       </c>
-      <c r="L9" s="33">
-        <v>0</v>
-      </c>
+      <c r="L9" s="17">
+        <v>0</v>
+      </c>
+      <c r="M9" s="33">
+        <v>0</v>
+      </c>
+      <c r="S9" s="1"/>
     </row>
     <row r="10" spans="1:36" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="40"/>
@@ -1804,7 +1818,9 @@
       <c r="I10" s="41"/>
       <c r="J10" s="41"/>
       <c r="K10" s="41"/>
-      <c r="L10" s="42"/>
+      <c r="L10" s="41"/>
+      <c r="M10" s="42"/>
+      <c r="S10" s="1"/>
     </row>
     <row r="11" spans="1:36" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
@@ -1840,9 +1856,13 @@
       <c r="K11" s="18">
         <v>0</v>
       </c>
-      <c r="L11" s="32">
-        <v>0</v>
-      </c>
+      <c r="L11" s="18">
+        <v>0</v>
+      </c>
+      <c r="M11" s="32">
+        <v>0</v>
+      </c>
+      <c r="S11" s="1"/>
     </row>
     <row r="12" spans="1:36" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
@@ -1878,16 +1898,19 @@
       <c r="K12" s="18">
         <v>0</v>
       </c>
-      <c r="L12" s="32">
-        <v>0</v>
-      </c>
-      <c r="N12" s="70" t="s">
+      <c r="L12" s="18">
+        <v>0</v>
+      </c>
+      <c r="M12" s="32">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="68" t="s">
         <v>38</v>
       </c>
-      <c r="O12" s="71"/>
-      <c r="P12" s="71"/>
-      <c r="Q12" s="71"/>
-      <c r="R12" s="72"/>
+      <c r="R12" s="75"/>
+      <c r="S12" s="75"/>
+      <c r="T12" s="75"/>
+      <c r="U12" s="76"/>
     </row>
     <row r="13" spans="1:36" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
@@ -1923,14 +1946,17 @@
       <c r="K13" s="18">
         <v>0</v>
       </c>
-      <c r="L13" s="32">
-        <v>0</v>
-      </c>
-      <c r="N13" s="73"/>
-      <c r="O13" s="74"/>
-      <c r="P13" s="74"/>
-      <c r="Q13" s="74"/>
-      <c r="R13" s="75"/>
+      <c r="L13" s="18">
+        <v>0</v>
+      </c>
+      <c r="M13" s="32">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="77"/>
+      <c r="R13" s="78"/>
+      <c r="S13" s="78"/>
+      <c r="T13" s="78"/>
+      <c r="U13" s="79"/>
     </row>
     <row r="14" spans="1:36" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="9" t="s">
@@ -1966,14 +1992,17 @@
       <c r="K14" s="18">
         <v>0</v>
       </c>
-      <c r="L14" s="32">
-        <v>0</v>
-      </c>
-      <c r="N14" s="76"/>
-      <c r="O14" s="77"/>
-      <c r="P14" s="77"/>
-      <c r="Q14" s="77"/>
-      <c r="R14" s="78"/>
+      <c r="L14" s="18">
+        <v>0</v>
+      </c>
+      <c r="M14" s="32">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="80"/>
+      <c r="R14" s="81"/>
+      <c r="S14" s="81"/>
+      <c r="T14" s="81"/>
+      <c r="U14" s="82"/>
     </row>
     <row r="15" spans="1:36" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="22" t="s">
@@ -2009,7 +2038,10 @@
       <c r="K15" s="18">
         <v>0</v>
       </c>
-      <c r="L15" s="32">
+      <c r="L15" s="18">
+        <v>0</v>
+      </c>
+      <c r="M15" s="32">
         <v>0</v>
       </c>
     </row>
@@ -2025,9 +2057,10 @@
       <c r="I16" s="41"/>
       <c r="J16" s="41"/>
       <c r="K16" s="41"/>
-      <c r="L16" s="42"/>
-    </row>
-    <row r="17" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L16" s="41"/>
+      <c r="M16" s="42"/>
+    </row>
+    <row r="17" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="28" t="s">
         <v>18</v>
       </c>
@@ -2061,11 +2094,14 @@
       <c r="K17" s="18">
         <v>0</v>
       </c>
-      <c r="L17" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L17" s="18">
+        <v>1</v>
+      </c>
+      <c r="M17" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="14" t="s">
         <v>19</v>
       </c>
@@ -2099,11 +2135,14 @@
       <c r="K18" s="18">
         <v>1</v>
       </c>
-      <c r="L18" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L18" s="18">
+        <v>0</v>
+      </c>
+      <c r="M18" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="10" t="s">
         <v>20</v>
       </c>
@@ -2137,11 +2176,14 @@
       <c r="K19" s="18">
         <v>0</v>
       </c>
-      <c r="L19" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L19" s="18">
+        <v>0</v>
+      </c>
+      <c r="M19" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="13" t="s">
         <v>21</v>
       </c>
@@ -2175,11 +2217,14 @@
       <c r="K20" s="18">
         <v>0</v>
       </c>
-      <c r="L20" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L20" s="18">
+        <v>0</v>
+      </c>
+      <c r="M20" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="25" t="s">
         <v>22</v>
       </c>
@@ -2213,11 +2258,14 @@
       <c r="K21" s="16">
         <v>0</v>
       </c>
-      <c r="L21" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L21" s="16">
+        <v>0</v>
+      </c>
+      <c r="M21" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="40"/>
       <c r="B22" s="41"/>
       <c r="C22" s="41"/>
@@ -2229,9 +2277,10 @@
       <c r="I22" s="41"/>
       <c r="J22" s="41"/>
       <c r="K22" s="41"/>
-      <c r="L22" s="42"/>
-    </row>
-    <row r="23" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L22" s="41"/>
+      <c r="M22" s="42"/>
+    </row>
+    <row r="23" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="28" t="s">
         <v>23</v>
       </c>
@@ -2265,11 +2314,14 @@
       <c r="K23" s="18">
         <v>0</v>
       </c>
-      <c r="L23" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L23" s="18">
+        <v>0</v>
+      </c>
+      <c r="M23" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="10" t="s">
         <v>24</v>
       </c>
@@ -2303,11 +2355,14 @@
       <c r="K24" s="18">
         <v>0</v>
       </c>
-      <c r="L24" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L24" s="18">
+        <v>0</v>
+      </c>
+      <c r="M24" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="10" t="s">
         <v>25</v>
       </c>
@@ -2341,11 +2396,14 @@
       <c r="K25" s="18">
         <v>0</v>
       </c>
-      <c r="L25" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L25" s="18">
+        <v>0</v>
+      </c>
+      <c r="M25" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="10" t="s">
         <v>26</v>
       </c>
@@ -2379,11 +2437,14 @@
       <c r="K26" s="18">
         <v>0</v>
       </c>
-      <c r="L26" s="32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L26" s="18">
+        <v>0</v>
+      </c>
+      <c r="M26" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="10" t="s">
         <v>27</v>
       </c>
@@ -2417,11 +2478,14 @@
       <c r="K27" s="18">
         <v>0</v>
       </c>
-      <c r="L27" s="32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L27" s="18">
+        <v>1</v>
+      </c>
+      <c r="M27" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="10" t="s">
         <v>28</v>
       </c>
@@ -2455,11 +2519,14 @@
       <c r="K28" s="15">
         <v>1</v>
       </c>
-      <c r="L28" s="32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L28" s="15">
+        <v>0</v>
+      </c>
+      <c r="M28" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="10" t="s">
         <v>29</v>
       </c>
@@ -2493,11 +2560,14 @@
       <c r="K29" s="16">
         <v>0</v>
       </c>
-      <c r="L29" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L29" s="16">
+        <v>1</v>
+      </c>
+      <c r="M29" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="36" t="s">
         <v>30</v>
       </c>
@@ -2531,19 +2601,22 @@
       <c r="K30" s="35">
         <v>1</v>
       </c>
-      <c r="L30" s="34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+      <c r="L30" s="35">
+        <v>0</v>
+      </c>
+      <c r="M30" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="S1:U1"/>
+    <mergeCell ref="Q12:U14"/>
     <mergeCell ref="A1:A2"/>
-    <mergeCell ref="G1:L1"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="N12:R14"/>
     <mergeCell ref="B1:F2"/>
+    <mergeCell ref="G1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>